<commit_message>
add netto da pagare
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -403,45 +403,50 @@
       </c>
       <c r="J1" t="inlineStr">
         <is>
+          <t>netto_da_pagare</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
           <t>par_a_prec</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>par_godute</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>par_saldo</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>par_spett</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>periodo</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>scatti</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>sup_ass</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>superm</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>totale_retributivo</t>
         </is>
@@ -457,16 +462,19 @@
       <c r="H2" t="n">
         <v>1634.56</v>
       </c>
-      <c r="O2" t="n">
-        <v>0</v>
+      <c r="J2" t="n">
+        <v>255</v>
       </c>
       <c r="P2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="n">
         <v>85.87</v>
       </c>
-      <c r="Q2" t="n">
-        <v>0</v>
-      </c>
       <c r="R2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S2" t="n">
         <v>1730.76</v>
       </c>
     </row>
@@ -480,16 +488,19 @@
       <c r="H3" t="n">
         <v>1634.56</v>
       </c>
-      <c r="O3" t="n">
-        <v>0</v>
+      <c r="J3" t="n">
+        <v>1339</v>
       </c>
       <c r="P3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q3" t="n">
         <v>85.87</v>
       </c>
-      <c r="Q3" t="n">
-        <v>0</v>
-      </c>
       <c r="R3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S3" t="n">
         <v>1730.76</v>
       </c>
     </row>
@@ -503,16 +514,19 @@
       <c r="H4" t="n">
         <v>1634.56</v>
       </c>
-      <c r="O4" t="n">
-        <v>0</v>
+      <c r="J4" t="n">
+        <v>1695</v>
       </c>
       <c r="P4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q4" t="n">
         <v>85.87</v>
       </c>
-      <c r="Q4" t="n">
-        <v>0</v>
-      </c>
       <c r="R4" t="n">
+        <v>0</v>
+      </c>
+      <c r="S4" t="n">
         <v>1730.76</v>
       </c>
     </row>
@@ -526,16 +540,19 @@
       <c r="H5" t="n">
         <v>1634.56</v>
       </c>
-      <c r="O5" t="n">
-        <v>0</v>
+      <c r="J5" t="n">
+        <v>1342</v>
       </c>
       <c r="P5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q5" t="n">
         <v>85.87</v>
       </c>
-      <c r="Q5" t="n">
-        <v>0</v>
-      </c>
       <c r="R5" t="n">
+        <v>0</v>
+      </c>
+      <c r="S5" t="n">
         <v>1730.76</v>
       </c>
     </row>
@@ -549,16 +566,19 @@
       <c r="H6" t="n">
         <v>1634.56</v>
       </c>
-      <c r="O6" t="n">
-        <v>0</v>
+      <c r="J6" t="n">
+        <v>755</v>
       </c>
       <c r="P6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q6" t="n">
         <v>85.87</v>
       </c>
-      <c r="Q6" t="n">
-        <v>0</v>
-      </c>
       <c r="R6" t="n">
+        <v>0</v>
+      </c>
+      <c r="S6" t="n">
         <v>1730.76</v>
       </c>
     </row>
@@ -572,16 +592,19 @@
       <c r="H7" t="n">
         <v>1634.56</v>
       </c>
-      <c r="O7" t="n">
-        <v>0</v>
+      <c r="J7" t="n">
+        <v>402</v>
       </c>
       <c r="P7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q7" t="n">
         <v>85.87</v>
       </c>
-      <c r="Q7" t="n">
-        <v>0</v>
-      </c>
       <c r="R7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S7" t="n">
         <v>1730.76</v>
       </c>
     </row>
@@ -595,16 +618,19 @@
       <c r="H8" t="n">
         <v>1679.89</v>
       </c>
-      <c r="O8" t="n">
-        <v>0</v>
+      <c r="J8" t="n">
+        <v>1271</v>
       </c>
       <c r="P8" t="n">
-        <v>50.87</v>
+        <v>0</v>
       </c>
       <c r="Q8" t="n">
-        <v>0</v>
+        <v>50.87</v>
       </c>
       <c r="R8" t="n">
+        <v>0</v>
+      </c>
+      <c r="S8" t="n">
         <v>1730.76</v>
       </c>
     </row>
@@ -618,16 +644,19 @@
       <c r="H9" t="n">
         <v>1679.89</v>
       </c>
-      <c r="O9" t="n">
-        <v>0</v>
+      <c r="J9" t="n">
+        <v>1306</v>
       </c>
       <c r="P9" t="n">
-        <v>50.87</v>
+        <v>0</v>
       </c>
       <c r="Q9" t="n">
-        <v>0</v>
+        <v>50.87</v>
       </c>
       <c r="R9" t="n">
+        <v>0</v>
+      </c>
+      <c r="S9" t="n">
         <v>1730.76</v>
       </c>
     </row>
@@ -641,16 +670,19 @@
       <c r="H10" t="n">
         <v>1679.89</v>
       </c>
-      <c r="O10" t="n">
-        <v>0</v>
+      <c r="J10" t="n">
+        <v>1264</v>
       </c>
       <c r="P10" t="n">
-        <v>50.87</v>
+        <v>0</v>
       </c>
       <c r="Q10" t="n">
-        <v>0</v>
+        <v>50.87</v>
       </c>
       <c r="R10" t="n">
+        <v>0</v>
+      </c>
+      <c r="S10" t="n">
         <v>1730.76</v>
       </c>
     </row>
@@ -664,16 +696,19 @@
       <c r="H11" t="n">
         <v>1679.89</v>
       </c>
-      <c r="O11" t="n">
-        <v>0</v>
+      <c r="J11" t="n">
+        <v>1262</v>
       </c>
       <c r="P11" t="n">
-        <v>50.87</v>
+        <v>0</v>
       </c>
       <c r="Q11" t="n">
-        <v>0</v>
+        <v>50.87</v>
       </c>
       <c r="R11" t="n">
+        <v>0</v>
+      </c>
+      <c r="S11" t="n">
         <v>1730.76</v>
       </c>
     </row>
@@ -687,16 +722,19 @@
       <c r="H12" t="n">
         <v>1679.89</v>
       </c>
-      <c r="O12" t="n">
-        <v>0</v>
+      <c r="J12" t="n">
+        <v>2472</v>
       </c>
       <c r="P12" t="n">
-        <v>50.87</v>
+        <v>0</v>
       </c>
       <c r="Q12" t="n">
-        <v>0</v>
+        <v>50.87</v>
       </c>
       <c r="R12" t="n">
+        <v>0</v>
+      </c>
+      <c r="S12" t="n">
         <v>1730.76</v>
       </c>
     </row>
@@ -710,16 +748,19 @@
       <c r="H13" t="n">
         <v>1679.89</v>
       </c>
-      <c r="O13" t="n">
-        <v>0</v>
+      <c r="J13" t="n">
+        <v>1259</v>
       </c>
       <c r="P13" t="n">
-        <v>50.87</v>
+        <v>0</v>
       </c>
       <c r="Q13" t="n">
-        <v>0</v>
+        <v>50.87</v>
       </c>
       <c r="R13" t="n">
+        <v>0</v>
+      </c>
+      <c r="S13" t="n">
         <v>1730.76</v>
       </c>
     </row>
@@ -733,16 +774,19 @@
       <c r="H14" t="n">
         <v>1679.89</v>
       </c>
-      <c r="O14" t="n">
-        <v>0</v>
+      <c r="J14" t="n">
+        <v>1306</v>
       </c>
       <c r="P14" t="n">
-        <v>50.87</v>
+        <v>0</v>
       </c>
       <c r="Q14" t="n">
-        <v>0</v>
+        <v>50.87</v>
       </c>
       <c r="R14" t="n">
+        <v>0</v>
+      </c>
+      <c r="S14" t="n">
         <v>1730.76</v>
       </c>
     </row>
@@ -756,16 +800,19 @@
       <c r="H15" t="n">
         <v>1679.89</v>
       </c>
-      <c r="O15" t="n">
-        <v>0</v>
+      <c r="J15" t="n">
+        <v>1262</v>
       </c>
       <c r="P15" t="n">
         <v>0</v>
       </c>
       <c r="Q15" t="n">
-        <v>50.87</v>
+        <v>0</v>
       </c>
       <c r="R15" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S15" t="n">
         <v>1730.76</v>
       </c>
     </row>
@@ -779,16 +826,19 @@
       <c r="H16" t="n">
         <v>1679.89</v>
       </c>
-      <c r="O16" t="n">
-        <v>0</v>
+      <c r="J16" t="n">
+        <v>1260</v>
       </c>
       <c r="P16" t="n">
         <v>0</v>
       </c>
       <c r="Q16" t="n">
-        <v>50.87</v>
+        <v>0</v>
       </c>
       <c r="R16" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S16" t="n">
         <v>1730.76</v>
       </c>
     </row>
@@ -802,16 +852,19 @@
       <c r="H17" t="n">
         <v>1679.89</v>
       </c>
-      <c r="O17" t="n">
-        <v>0</v>
+      <c r="J17" t="n">
+        <v>1963</v>
       </c>
       <c r="P17" t="n">
         <v>0</v>
       </c>
       <c r="Q17" t="n">
-        <v>50.87</v>
+        <v>0</v>
       </c>
       <c r="R17" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S17" t="n">
         <v>1730.76</v>
       </c>
     </row>
@@ -825,16 +878,19 @@
       <c r="H18" t="n">
         <v>1679.89</v>
       </c>
-      <c r="O18" t="n">
-        <v>0</v>
+      <c r="J18" t="n">
+        <v>1960</v>
       </c>
       <c r="P18" t="n">
         <v>0</v>
       </c>
       <c r="Q18" t="n">
-        <v>50.87</v>
+        <v>0</v>
       </c>
       <c r="R18" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S18" t="n">
         <v>1730.76</v>
       </c>
     </row>
@@ -848,16 +904,19 @@
       <c r="H19" t="n">
         <v>1679.89</v>
       </c>
-      <c r="O19" t="n">
-        <v>0</v>
+      <c r="J19" t="n">
+        <v>2104</v>
       </c>
       <c r="P19" t="n">
         <v>0</v>
       </c>
       <c r="Q19" t="n">
-        <v>50.87</v>
+        <v>0</v>
       </c>
       <c r="R19" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S19" t="n">
         <v>1730.76</v>
       </c>
     </row>
@@ -871,16 +930,19 @@
       <c r="H20" t="n">
         <v>1679.89</v>
       </c>
-      <c r="O20" t="n">
-        <v>0</v>
+      <c r="J20" t="n">
+        <v>1193</v>
       </c>
       <c r="P20" t="n">
         <v>0</v>
       </c>
       <c r="Q20" t="n">
-        <v>50.87</v>
+        <v>0</v>
       </c>
       <c r="R20" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S20" t="n">
         <v>1730.76</v>
       </c>
     </row>
@@ -894,16 +956,19 @@
       <c r="H21" t="n">
         <v>1724.89</v>
       </c>
-      <c r="O21" t="n">
-        <v>0</v>
+      <c r="J21" t="n">
+        <v>1861</v>
       </c>
       <c r="P21" t="n">
         <v>0</v>
       </c>
       <c r="Q21" t="n">
-        <v>50.87</v>
+        <v>0</v>
       </c>
       <c r="R21" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S21" t="n">
         <v>1775.76</v>
       </c>
     </row>
@@ -917,16 +982,19 @@
       <c r="H22" t="n">
         <v>1724.89</v>
       </c>
-      <c r="O22" t="n">
-        <v>0</v>
+      <c r="J22" t="n">
+        <v>2210</v>
       </c>
       <c r="P22" t="n">
         <v>0</v>
       </c>
       <c r="Q22" t="n">
-        <v>50.87</v>
+        <v>0</v>
       </c>
       <c r="R22" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S22" t="n">
         <v>1775.76</v>
       </c>
     </row>
@@ -940,16 +1008,19 @@
       <c r="H23" t="n">
         <v>1724.89</v>
       </c>
-      <c r="O23" t="n">
-        <v>0</v>
+      <c r="J23" t="n">
+        <v>2130</v>
       </c>
       <c r="P23" t="n">
         <v>0</v>
       </c>
       <c r="Q23" t="n">
-        <v>50.87</v>
+        <v>0</v>
       </c>
       <c r="R23" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S23" t="n">
         <v>1775.76</v>
       </c>
     </row>
@@ -963,16 +1034,19 @@
       <c r="H24" t="n">
         <v>1847.11</v>
       </c>
-      <c r="O24" t="n">
-        <v>0</v>
+      <c r="J24" t="n">
+        <v>3158</v>
       </c>
       <c r="P24" t="n">
         <v>0</v>
       </c>
       <c r="Q24" t="n">
-        <v>50.87</v>
+        <v>0</v>
       </c>
       <c r="R24" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S24" t="n">
         <v>1897.98</v>
       </c>
     </row>
@@ -986,16 +1060,19 @@
       <c r="H25" t="n">
         <v>1847.11</v>
       </c>
-      <c r="O25" t="n">
-        <v>0</v>
+      <c r="J25" t="n">
+        <v>2141</v>
       </c>
       <c r="P25" t="n">
         <v>0</v>
       </c>
       <c r="Q25" t="n">
-        <v>50.87</v>
+        <v>0</v>
       </c>
       <c r="R25" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S25" t="n">
         <v>1897.98</v>
       </c>
     </row>
@@ -1009,16 +1086,19 @@
       <c r="H26" t="n">
         <v>1847.11</v>
       </c>
-      <c r="O26" t="n">
-        <v>0</v>
+      <c r="J26" t="n">
+        <v>2155</v>
       </c>
       <c r="P26" t="n">
         <v>0</v>
       </c>
       <c r="Q26" t="n">
-        <v>50.87</v>
+        <v>0</v>
       </c>
       <c r="R26" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S26" t="n">
         <v>1897.98</v>
       </c>
     </row>
@@ -1032,16 +1112,19 @@
       <c r="H27" t="n">
         <v>1847.11</v>
       </c>
-      <c r="O27" t="n">
-        <v>0</v>
+      <c r="J27" t="n">
+        <v>2074</v>
       </c>
       <c r="P27" t="n">
         <v>0</v>
       </c>
       <c r="Q27" t="n">
-        <v>50.87</v>
+        <v>0</v>
       </c>
       <c r="R27" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S27" t="n">
         <v>1897.98</v>
       </c>
     </row>
@@ -1055,16 +1138,19 @@
       <c r="H28" t="n">
         <v>1847.11</v>
       </c>
-      <c r="O28" t="n">
-        <v>0</v>
+      <c r="J28" t="n">
+        <v>2083</v>
       </c>
       <c r="P28" t="n">
         <v>0</v>
       </c>
       <c r="Q28" t="n">
-        <v>50.87</v>
+        <v>0</v>
       </c>
       <c r="R28" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S28" t="n">
         <v>1897.98</v>
       </c>
     </row>
@@ -1078,16 +1164,19 @@
       <c r="H29" t="n">
         <v>1847.11</v>
       </c>
-      <c r="O29" t="n">
+      <c r="J29" t="n">
+        <v>1928</v>
+      </c>
+      <c r="P29" t="n">
         <v>32.43</v>
       </c>
-      <c r="P29" t="n">
-        <v>0</v>
-      </c>
       <c r="Q29" t="n">
-        <v>50.87</v>
+        <v>0</v>
       </c>
       <c r="R29" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S29" t="n">
         <v>1930.41</v>
       </c>
     </row>
@@ -1101,16 +1190,19 @@
       <c r="H30" t="n">
         <v>1847.11</v>
       </c>
-      <c r="O30" t="n">
+      <c r="J30" t="n">
+        <v>1976</v>
+      </c>
+      <c r="P30" t="n">
         <v>32.43</v>
       </c>
-      <c r="P30" t="n">
-        <v>0</v>
-      </c>
       <c r="Q30" t="n">
-        <v>50.87</v>
+        <v>0</v>
       </c>
       <c r="R30" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S30" t="n">
         <v>1930.41</v>
       </c>
     </row>
@@ -1124,16 +1216,19 @@
       <c r="H31" t="n">
         <v>1847.11</v>
       </c>
-      <c r="O31" t="n">
+      <c r="J31" t="n">
+        <v>2111</v>
+      </c>
+      <c r="P31" t="n">
         <v>32.43</v>
       </c>
-      <c r="P31" t="n">
-        <v>0</v>
-      </c>
       <c r="Q31" t="n">
-        <v>50.87</v>
+        <v>0</v>
       </c>
       <c r="R31" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S31" t="n">
         <v>1930.41</v>
       </c>
     </row>
@@ -1147,16 +1242,19 @@
       <c r="H32" t="n">
         <v>1847.11</v>
       </c>
-      <c r="O32" t="n">
+      <c r="J32" t="n">
+        <v>2465</v>
+      </c>
+      <c r="P32" t="n">
         <v>32.43</v>
       </c>
-      <c r="P32" t="n">
-        <v>0</v>
-      </c>
       <c r="Q32" t="n">
-        <v>50.87</v>
+        <v>0</v>
       </c>
       <c r="R32" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S32" t="n">
         <v>1930.41</v>
       </c>
     </row>
@@ -1170,16 +1268,19 @@
       <c r="H33" t="n">
         <v>1847.11</v>
       </c>
-      <c r="O33" t="n">
+      <c r="J33" t="n">
+        <v>1326</v>
+      </c>
+      <c r="P33" t="n">
         <v>32.43</v>
       </c>
-      <c r="P33" t="n">
-        <v>0</v>
-      </c>
       <c r="Q33" t="n">
-        <v>50.87</v>
+        <v>0</v>
       </c>
       <c r="R33" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S33" t="n">
         <v>1930.41</v>
       </c>
     </row>
@@ -1193,16 +1294,19 @@
       <c r="H34" t="n">
         <v>1902.42</v>
       </c>
-      <c r="O34" t="n">
+      <c r="J34" t="n">
+        <v>2300</v>
+      </c>
+      <c r="P34" t="n">
         <v>32.43</v>
       </c>
-      <c r="P34" t="n">
-        <v>0</v>
-      </c>
       <c r="Q34" t="n">
-        <v>50.87</v>
+        <v>0</v>
       </c>
       <c r="R34" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S34" t="n">
         <v>1985.72</v>
       </c>
     </row>
@@ -1216,16 +1320,19 @@
       <c r="H35" t="n">
         <v>1902.42</v>
       </c>
-      <c r="O35" t="n">
+      <c r="J35" t="n">
+        <v>2412</v>
+      </c>
+      <c r="P35" t="n">
         <v>32.43</v>
       </c>
-      <c r="P35" t="n">
-        <v>0</v>
-      </c>
       <c r="Q35" t="n">
-        <v>50.87</v>
+        <v>0</v>
       </c>
       <c r="R35" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S35" t="n">
         <v>1985.72</v>
       </c>
     </row>
@@ -1239,16 +1346,19 @@
       <c r="H36" t="n">
         <v>1902.42</v>
       </c>
-      <c r="O36" t="n">
+      <c r="J36" t="n">
+        <v>2123</v>
+      </c>
+      <c r="P36" t="n">
         <v>32.43</v>
       </c>
-      <c r="P36" t="n">
-        <v>0</v>
-      </c>
       <c r="Q36" t="n">
-        <v>50.87</v>
+        <v>0</v>
       </c>
       <c r="R36" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S36" t="n">
         <v>1985.72</v>
       </c>
     </row>
@@ -1262,16 +1372,19 @@
       <c r="H37" t="n">
         <v>1902.42</v>
       </c>
-      <c r="O37" t="n">
+      <c r="J37" t="n">
+        <v>2108</v>
+      </c>
+      <c r="P37" t="n">
         <v>32.43</v>
       </c>
-      <c r="P37" t="n">
-        <v>0</v>
-      </c>
       <c r="Q37" t="n">
-        <v>50.87</v>
+        <v>0</v>
       </c>
       <c r="R37" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S37" t="n">
         <v>1985.72</v>
       </c>
     </row>
@@ -1285,16 +1398,19 @@
       <c r="H38" t="n">
         <v>1902.42</v>
       </c>
-      <c r="O38" t="n">
+      <c r="J38" t="n">
+        <v>2119</v>
+      </c>
+      <c r="P38" t="n">
         <v>32.43</v>
       </c>
-      <c r="P38" t="n">
-        <v>0</v>
-      </c>
       <c r="Q38" t="n">
-        <v>50.87</v>
+        <v>0</v>
       </c>
       <c r="R38" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S38" t="n">
         <v>1985.72</v>
       </c>
     </row>
@@ -1308,16 +1424,19 @@
       <c r="H39" t="n">
         <v>1902.42</v>
       </c>
-      <c r="O39" t="n">
+      <c r="J39" t="n">
+        <v>2143</v>
+      </c>
+      <c r="P39" t="n">
         <v>32.43</v>
       </c>
-      <c r="P39" t="n">
-        <v>0</v>
-      </c>
       <c r="Q39" t="n">
-        <v>50.87</v>
+        <v>0</v>
       </c>
       <c r="R39" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S39" t="n">
         <v>1985.72</v>
       </c>
     </row>
@@ -1331,16 +1450,19 @@
       <c r="H40" t="n">
         <v>1902.42</v>
       </c>
-      <c r="O40" t="n">
+      <c r="J40" t="n">
+        <v>2145</v>
+      </c>
+      <c r="P40" t="n">
         <v>32.43</v>
       </c>
-      <c r="P40" t="n">
-        <v>0</v>
-      </c>
       <c r="Q40" t="n">
-        <v>50.87</v>
+        <v>0</v>
       </c>
       <c r="R40" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S40" t="n">
         <v>1985.72</v>
       </c>
     </row>
@@ -1354,16 +1476,19 @@
       <c r="H41" t="n">
         <v>1902.42</v>
       </c>
-      <c r="O41" t="n">
+      <c r="J41" t="n">
+        <v>2144</v>
+      </c>
+      <c r="P41" t="n">
         <v>32.43</v>
       </c>
-      <c r="P41" t="n">
-        <v>0</v>
-      </c>
       <c r="Q41" t="n">
-        <v>50.87</v>
+        <v>0</v>
       </c>
       <c r="R41" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S41" t="n">
         <v>1985.72</v>
       </c>
     </row>
@@ -1377,16 +1502,19 @@
       <c r="H42" t="n">
         <v>1902.42</v>
       </c>
-      <c r="O42" t="n">
+      <c r="J42" t="n">
+        <v>2163</v>
+      </c>
+      <c r="P42" t="n">
         <v>32.43</v>
       </c>
-      <c r="P42" t="n">
-        <v>0</v>
-      </c>
       <c r="Q42" t="n">
-        <v>50.87</v>
+        <v>0</v>
       </c>
       <c r="R42" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S42" t="n">
         <v>1985.72</v>
       </c>
     </row>
@@ -1400,16 +1528,19 @@
       <c r="H43" t="n">
         <v>1902.42</v>
       </c>
-      <c r="O43" t="n">
+      <c r="J43" t="n">
+        <v>2414</v>
+      </c>
+      <c r="P43" t="n">
         <v>32.43</v>
       </c>
-      <c r="P43" t="n">
-        <v>0</v>
-      </c>
       <c r="Q43" t="n">
-        <v>50.87</v>
+        <v>0</v>
       </c>
       <c r="R43" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S43" t="n">
         <v>1985.72</v>
       </c>
     </row>
@@ -1423,16 +1554,19 @@
       <c r="H44" t="n">
         <v>1902.42</v>
       </c>
-      <c r="O44" t="n">
+      <c r="J44" t="n">
+        <v>2276</v>
+      </c>
+      <c r="P44" t="n">
         <v>32.43</v>
       </c>
-      <c r="P44" t="n">
-        <v>0</v>
-      </c>
       <c r="Q44" t="n">
-        <v>50.87</v>
+        <v>0</v>
       </c>
       <c r="R44" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S44" t="n">
         <v>1985.72</v>
       </c>
     </row>
@@ -1446,16 +1580,19 @@
       <c r="H45" t="n">
         <v>1902.42</v>
       </c>
-      <c r="O45" t="n">
+      <c r="J45" t="n">
+        <v>2530</v>
+      </c>
+      <c r="P45" t="n">
         <v>32.43</v>
       </c>
-      <c r="P45" t="n">
-        <v>0</v>
-      </c>
       <c r="Q45" t="n">
-        <v>50.87</v>
+        <v>0</v>
       </c>
       <c r="R45" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S45" t="n">
         <v>1985.72</v>
       </c>
     </row>
@@ -1469,16 +1606,19 @@
       <c r="H46" t="n">
         <v>1902.42</v>
       </c>
-      <c r="O46" t="n">
+      <c r="J46" t="n">
+        <v>1362</v>
+      </c>
+      <c r="P46" t="n">
         <v>32.43</v>
       </c>
-      <c r="P46" t="n">
-        <v>0</v>
-      </c>
       <c r="Q46" t="n">
-        <v>50.87</v>
+        <v>0</v>
       </c>
       <c r="R46" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S46" t="n">
         <v>1985.72</v>
       </c>
     </row>
@@ -1492,16 +1632,19 @@
       <c r="H47" t="n">
         <v>1902.42</v>
       </c>
-      <c r="O47" t="n">
+      <c r="J47" t="n">
+        <v>1970</v>
+      </c>
+      <c r="P47" t="n">
         <v>32.43</v>
       </c>
-      <c r="P47" t="n">
-        <v>0</v>
-      </c>
       <c r="Q47" t="n">
-        <v>50.87</v>
+        <v>0</v>
       </c>
       <c r="R47" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S47" t="n">
         <v>1985.72</v>
       </c>
     </row>
@@ -1515,16 +1658,19 @@
       <c r="H48" t="n">
         <v>1902.42</v>
       </c>
-      <c r="O48" t="n">
+      <c r="J48" t="n">
+        <v>2189</v>
+      </c>
+      <c r="P48" t="n">
         <v>32.43</v>
       </c>
-      <c r="P48" t="n">
-        <v>0</v>
-      </c>
       <c r="Q48" t="n">
-        <v>50.87</v>
+        <v>0</v>
       </c>
       <c r="R48" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S48" t="n">
         <v>1985.72</v>
       </c>
     </row>
@@ -1538,16 +1684,19 @@
       <c r="H49" t="n">
         <v>1902.42</v>
       </c>
-      <c r="O49" t="n">
+      <c r="J49" t="n">
+        <v>2793</v>
+      </c>
+      <c r="P49" t="n">
         <v>32.43</v>
       </c>
-      <c r="P49" t="n">
-        <v>0</v>
-      </c>
       <c r="Q49" t="n">
-        <v>50.87</v>
+        <v>0</v>
       </c>
       <c r="R49" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S49" t="n">
         <v>1985.72</v>
       </c>
     </row>
@@ -1561,16 +1710,19 @@
       <c r="H50" t="n">
         <v>1902.42</v>
       </c>
-      <c r="O50" t="n">
+      <c r="J50" t="n">
+        <v>2191</v>
+      </c>
+      <c r="P50" t="n">
         <v>32.43</v>
       </c>
-      <c r="P50" t="n">
-        <v>0</v>
-      </c>
       <c r="Q50" t="n">
-        <v>50.87</v>
+        <v>0</v>
       </c>
       <c r="R50" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S50" t="n">
         <v>1985.72</v>
       </c>
     </row>
@@ -1584,16 +1736,19 @@
       <c r="H51" t="n">
         <v>1902.42</v>
       </c>
-      <c r="O51" t="n">
+      <c r="J51" t="n">
+        <v>2194</v>
+      </c>
+      <c r="P51" t="n">
         <v>32.43</v>
       </c>
-      <c r="P51" t="n">
-        <v>0</v>
-      </c>
       <c r="Q51" t="n">
-        <v>50.87</v>
+        <v>0</v>
       </c>
       <c r="R51" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S51" t="n">
         <v>1985.72</v>
       </c>
     </row>
@@ -1607,16 +1762,19 @@
       <c r="H52" t="n">
         <v>1902.42</v>
       </c>
-      <c r="O52" t="n">
+      <c r="J52" t="n">
+        <v>2261</v>
+      </c>
+      <c r="P52" t="n">
         <v>32.43</v>
       </c>
-      <c r="P52" t="n">
-        <v>0</v>
-      </c>
       <c r="Q52" t="n">
-        <v>50.87</v>
+        <v>0</v>
       </c>
       <c r="R52" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S52" t="n">
         <v>1985.72</v>
       </c>
     </row>
@@ -1630,16 +1788,19 @@
       <c r="H53" t="n">
         <v>1902.42</v>
       </c>
-      <c r="O53" t="n">
+      <c r="J53" t="n">
+        <v>2837</v>
+      </c>
+      <c r="P53" t="n">
         <v>32.43</v>
       </c>
-      <c r="P53" t="n">
-        <v>0</v>
-      </c>
       <c r="Q53" t="n">
-        <v>50.87</v>
+        <v>0</v>
       </c>
       <c r="R53" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S53" t="n">
         <v>1985.72</v>
       </c>
     </row>
@@ -1653,16 +1814,19 @@
       <c r="H54" t="n">
         <v>1902.42</v>
       </c>
-      <c r="O54" t="n">
+      <c r="J54" t="n">
+        <v>2891</v>
+      </c>
+      <c r="P54" t="n">
         <v>32.43</v>
       </c>
-      <c r="P54" t="n">
-        <v>0</v>
-      </c>
       <c r="Q54" t="n">
-        <v>50.87</v>
+        <v>0</v>
       </c>
       <c r="R54" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S54" t="n">
         <v>1985.72</v>
       </c>
     </row>
@@ -1676,16 +1840,19 @@
       <c r="H55" t="n">
         <v>1902.42</v>
       </c>
-      <c r="O55" t="n">
+      <c r="J55" t="n">
+        <v>2655</v>
+      </c>
+      <c r="P55" t="n">
         <v>64.86</v>
       </c>
-      <c r="P55" t="n">
-        <v>0</v>
-      </c>
       <c r="Q55" t="n">
-        <v>50.87</v>
+        <v>0</v>
       </c>
       <c r="R55" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S55" t="n">
         <v>2018.15</v>
       </c>
     </row>
@@ -1699,16 +1866,19 @@
       <c r="H56" t="n">
         <v>1902.42</v>
       </c>
-      <c r="O56" t="n">
+      <c r="J56" t="n">
+        <v>2586</v>
+      </c>
+      <c r="P56" t="n">
         <v>64.86</v>
       </c>
-      <c r="P56" t="n">
-        <v>0</v>
-      </c>
       <c r="Q56" t="n">
-        <v>50.87</v>
+        <v>0</v>
       </c>
       <c r="R56" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S56" t="n">
         <v>2018.15</v>
       </c>
     </row>
@@ -1722,16 +1892,19 @@
       <c r="H57" t="n">
         <v>1902.42</v>
       </c>
-      <c r="O57" t="n">
+      <c r="J57" t="n">
+        <v>2763</v>
+      </c>
+      <c r="P57" t="n">
         <v>64.86</v>
       </c>
-      <c r="P57" t="n">
-        <v>0</v>
-      </c>
       <c r="Q57" t="n">
-        <v>50.87</v>
+        <v>0</v>
       </c>
       <c r="R57" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S57" t="n">
         <v>2018.15</v>
       </c>
     </row>
@@ -1745,16 +1918,19 @@
       <c r="H58" t="n">
         <v>1902.42</v>
       </c>
-      <c r="O58" t="n">
+      <c r="J58" t="n">
+        <v>2367</v>
+      </c>
+      <c r="P58" t="n">
         <v>64.86</v>
       </c>
-      <c r="P58" t="n">
-        <v>0</v>
-      </c>
       <c r="Q58" t="n">
-        <v>50.87</v>
+        <v>0</v>
       </c>
       <c r="R58" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S58" t="n">
         <v>2018.15</v>
       </c>
     </row>
@@ -1768,16 +1944,19 @@
       <c r="H59" t="n">
         <v>1902.42</v>
       </c>
-      <c r="O59" t="n">
+      <c r="J59" t="n">
+        <v>1383</v>
+      </c>
+      <c r="P59" t="n">
         <v>64.86</v>
       </c>
-      <c r="P59" t="n">
-        <v>0</v>
-      </c>
       <c r="Q59" t="n">
-        <v>50.87</v>
+        <v>0</v>
       </c>
       <c r="R59" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S59" t="n">
         <v>2018.15</v>
       </c>
     </row>
@@ -1791,16 +1970,19 @@
       <c r="H60" t="n">
         <v>1902.42</v>
       </c>
-      <c r="O60" t="n">
+      <c r="J60" t="n">
+        <v>2755</v>
+      </c>
+      <c r="P60" t="n">
         <v>64.86</v>
       </c>
-      <c r="P60" t="n">
-        <v>0</v>
-      </c>
       <c r="Q60" t="n">
-        <v>50.87</v>
+        <v>0</v>
       </c>
       <c r="R60" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S60" t="n">
         <v>2018.15</v>
       </c>
     </row>
@@ -1814,16 +1996,19 @@
       <c r="H61" t="n">
         <v>1902.42</v>
       </c>
-      <c r="O61" t="n">
+      <c r="J61" t="n">
+        <v>1895</v>
+      </c>
+      <c r="P61" t="n">
         <v>64.86</v>
       </c>
-      <c r="P61" t="n">
-        <v>674.16</v>
-      </c>
       <c r="Q61" t="n">
-        <v>50.87</v>
+        <v>674.16</v>
       </c>
       <c r="R61" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S61" t="n">
         <v>2692.31</v>
       </c>
     </row>
@@ -1837,16 +2022,19 @@
       <c r="H62" t="n">
         <v>1902.42</v>
       </c>
-      <c r="O62" t="n">
+      <c r="J62" t="n">
+        <v>2444</v>
+      </c>
+      <c r="P62" t="n">
         <v>64.86</v>
       </c>
-      <c r="P62" t="n">
-        <v>674.16</v>
-      </c>
       <c r="Q62" t="n">
-        <v>50.87</v>
+        <v>674.16</v>
       </c>
       <c r="R62" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S62" t="n">
         <v>2692.31</v>
       </c>
     </row>
@@ -1860,16 +2048,19 @@
       <c r="H63" t="n">
         <v>1902.42</v>
       </c>
-      <c r="O63" t="n">
+      <c r="J63" t="n">
+        <v>2375</v>
+      </c>
+      <c r="P63" t="n">
         <v>64.86</v>
       </c>
-      <c r="P63" t="n">
-        <v>674.16</v>
-      </c>
       <c r="Q63" t="n">
-        <v>50.87</v>
+        <v>674.16</v>
       </c>
       <c r="R63" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S63" t="n">
         <v>2692.31</v>
       </c>
     </row>
@@ -1883,16 +2074,19 @@
       <c r="H64" t="n">
         <v>1902.42</v>
       </c>
-      <c r="O64" t="n">
+      <c r="J64" t="n">
+        <v>2242</v>
+      </c>
+      <c r="P64" t="n">
         <v>64.86</v>
       </c>
-      <c r="P64" t="n">
-        <v>674.16</v>
-      </c>
       <c r="Q64" t="n">
-        <v>50.87</v>
+        <v>674.16</v>
       </c>
       <c r="R64" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S64" t="n">
         <v>2692.31</v>
       </c>
     </row>
@@ -1906,16 +2100,19 @@
       <c r="H65" t="n">
         <v>1904.32</v>
       </c>
-      <c r="O65" t="n">
+      <c r="J65" t="n">
+        <v>2209</v>
+      </c>
+      <c r="P65" t="n">
         <v>64.86</v>
       </c>
-      <c r="P65" t="n">
-        <v>674.16</v>
-      </c>
       <c r="Q65" t="n">
-        <v>50.87</v>
+        <v>674.16</v>
       </c>
       <c r="R65" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S65" t="n">
         <v>2694.21</v>
       </c>
     </row>
@@ -1929,16 +2126,19 @@
       <c r="H66" t="n">
         <v>1904.32</v>
       </c>
-      <c r="O66" t="n">
+      <c r="J66" t="n">
+        <v>2273</v>
+      </c>
+      <c r="P66" t="n">
         <v>64.86</v>
       </c>
-      <c r="P66" t="n">
-        <v>674.16</v>
-      </c>
       <c r="Q66" t="n">
-        <v>50.87</v>
+        <v>674.16</v>
       </c>
       <c r="R66" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S66" t="n">
         <v>2694.21</v>
       </c>
     </row>
@@ -1952,16 +2152,19 @@
       <c r="H67" t="n">
         <v>1904.32</v>
       </c>
-      <c r="O67" t="n">
+      <c r="J67" t="n">
+        <v>2001</v>
+      </c>
+      <c r="P67" t="n">
         <v>64.86</v>
       </c>
-      <c r="P67" t="n">
-        <v>674.16</v>
-      </c>
       <c r="Q67" t="n">
-        <v>50.87</v>
+        <v>674.16</v>
       </c>
       <c r="R67" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S67" t="n">
         <v>2694.21</v>
       </c>
     </row>
@@ -1975,16 +2178,19 @@
       <c r="H68" t="n">
         <v>1904.32</v>
       </c>
-      <c r="O68" t="n">
+      <c r="J68" t="n">
+        <v>1999</v>
+      </c>
+      <c r="P68" t="n">
         <v>64.86</v>
       </c>
-      <c r="P68" t="n">
-        <v>674.16</v>
-      </c>
       <c r="Q68" t="n">
-        <v>50.87</v>
+        <v>674.16</v>
       </c>
       <c r="R68" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S68" t="n">
         <v>2694.21</v>
       </c>
     </row>
@@ -1998,16 +2204,19 @@
       <c r="H69" t="n">
         <v>1904.32</v>
       </c>
-      <c r="O69" t="n">
+      <c r="J69" t="n">
+        <v>2001</v>
+      </c>
+      <c r="P69" t="n">
         <v>64.86</v>
       </c>
-      <c r="P69" t="n">
-        <v>674.16</v>
-      </c>
       <c r="Q69" t="n">
-        <v>50.87</v>
+        <v>674.16</v>
       </c>
       <c r="R69" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S69" t="n">
         <v>2694.21</v>
       </c>
     </row>
@@ -2021,16 +2230,19 @@
       <c r="H70" t="n">
         <v>1904.32</v>
       </c>
-      <c r="O70" t="n">
+      <c r="J70" t="n">
+        <v>1871</v>
+      </c>
+      <c r="P70" t="n">
         <v>64.86</v>
       </c>
-      <c r="P70" t="n">
-        <v>674.16</v>
-      </c>
       <c r="Q70" t="n">
-        <v>50.87</v>
+        <v>674.16</v>
       </c>
       <c r="R70" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S70" t="n">
         <v>2694.21</v>
       </c>
     </row>
@@ -2044,16 +2256,19 @@
       <c r="H71" t="n">
         <v>1904.32</v>
       </c>
-      <c r="O71" t="n">
+      <c r="J71" t="n">
+        <v>1838</v>
+      </c>
+      <c r="P71" t="n">
         <v>64.86</v>
       </c>
-      <c r="P71" t="n">
-        <v>674.16</v>
-      </c>
       <c r="Q71" t="n">
-        <v>50.87</v>
+        <v>674.16</v>
       </c>
       <c r="R71" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S71" t="n">
         <v>2694.21</v>
       </c>
     </row>
@@ -2067,16 +2282,19 @@
       <c r="H72" t="n">
         <v>1904.32</v>
       </c>
-      <c r="O72" t="n">
+      <c r="J72" t="n">
+        <v>1818</v>
+      </c>
+      <c r="P72" t="n">
         <v>64.86</v>
       </c>
-      <c r="P72" t="n">
-        <v>674.16</v>
-      </c>
       <c r="Q72" t="n">
-        <v>50.87</v>
+        <v>674.16</v>
       </c>
       <c r="R72" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S72" t="n">
         <v>2694.21</v>
       </c>
     </row>
@@ -2090,16 +2308,19 @@
       <c r="H73" t="n">
         <v>1904.32</v>
       </c>
-      <c r="O73" t="n">
+      <c r="J73" t="n">
+        <v>2050</v>
+      </c>
+      <c r="P73" t="n">
         <v>64.86</v>
       </c>
-      <c r="P73" t="n">
-        <v>674.16</v>
-      </c>
       <c r="Q73" t="n">
-        <v>50.87</v>
+        <v>674.16</v>
       </c>
       <c r="R73" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S73" t="n">
         <v>2694.21</v>
       </c>
     </row>
@@ -2113,16 +2334,19 @@
       <c r="H74" t="n">
         <v>1904.32</v>
       </c>
-      <c r="O74" t="n">
+      <c r="J74" t="n">
+        <v>2058</v>
+      </c>
+      <c r="P74" t="n">
         <v>64.86</v>
       </c>
-      <c r="P74" t="n">
-        <v>674.16</v>
-      </c>
       <c r="Q74" t="n">
-        <v>50.87</v>
+        <v>674.16</v>
       </c>
       <c r="R74" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S74" t="n">
         <v>2694.21</v>
       </c>
     </row>
@@ -2136,16 +2360,19 @@
       <c r="H75" t="n">
         <v>1904.32</v>
       </c>
-      <c r="O75" t="n">
+      <c r="J75" t="n">
+        <v>1977</v>
+      </c>
+      <c r="P75" t="n">
         <v>64.86</v>
       </c>
-      <c r="P75" t="n">
-        <v>674.16</v>
-      </c>
       <c r="Q75" t="n">
-        <v>50.87</v>
+        <v>674.16</v>
       </c>
       <c r="R75" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S75" t="n">
         <v>2694.21</v>
       </c>
     </row>
@@ -2159,16 +2386,19 @@
       <c r="H76" t="n">
         <v>1904.32</v>
       </c>
-      <c r="O76" t="n">
+      <c r="J76" t="n">
+        <v>1980</v>
+      </c>
+      <c r="P76" t="n">
         <v>64.86</v>
       </c>
-      <c r="P76" t="n">
-        <v>674.16</v>
-      </c>
       <c r="Q76" t="n">
-        <v>50.87</v>
+        <v>674.16</v>
       </c>
       <c r="R76" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S76" t="n">
         <v>2694.21</v>
       </c>
     </row>
@@ -2182,16 +2412,19 @@
       <c r="H77" t="n">
         <v>1904.32</v>
       </c>
-      <c r="O77" t="n">
+      <c r="J77" t="n">
+        <v>2071</v>
+      </c>
+      <c r="P77" t="n">
         <v>64.86</v>
       </c>
-      <c r="P77" t="n">
-        <v>674.16</v>
-      </c>
       <c r="Q77" t="n">
-        <v>50.87</v>
+        <v>674.16</v>
       </c>
       <c r="R77" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S77" t="n">
         <v>2694.21</v>
       </c>
     </row>
@@ -2205,16 +2438,19 @@
       <c r="H78" t="n">
         <v>1921.46</v>
       </c>
-      <c r="O78" t="n">
+      <c r="J78" t="n">
+        <v>3960</v>
+      </c>
+      <c r="P78" t="n">
         <v>64.86</v>
       </c>
-      <c r="P78" t="n">
-        <v>674.16</v>
-      </c>
       <c r="Q78" t="n">
-        <v>50.87</v>
+        <v>674.16</v>
       </c>
       <c r="R78" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S78" t="n">
         <v>2711.35</v>
       </c>
     </row>
@@ -2228,16 +2464,19 @@
       <c r="H79" t="n">
         <v>1921.46</v>
       </c>
-      <c r="O79" t="n">
+      <c r="J79" t="n">
+        <v>1929</v>
+      </c>
+      <c r="P79" t="n">
         <v>64.86</v>
       </c>
-      <c r="P79" t="n">
-        <v>674.16</v>
-      </c>
       <c r="Q79" t="n">
-        <v>50.87</v>
+        <v>674.16</v>
       </c>
       <c r="R79" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S79" t="n">
         <v>2711.35</v>
       </c>
     </row>
@@ -2251,16 +2490,19 @@
       <c r="H80" t="n">
         <v>1921.46</v>
       </c>
-      <c r="O80" t="n">
+      <c r="J80" t="n">
+        <v>2007</v>
+      </c>
+      <c r="P80" t="n">
         <v>64.86</v>
       </c>
-      <c r="P80" t="n">
-        <v>674.16</v>
-      </c>
       <c r="Q80" t="n">
-        <v>50.87</v>
+        <v>674.16</v>
       </c>
       <c r="R80" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S80" t="n">
         <v>2711.35</v>
       </c>
     </row>
@@ -2274,16 +2516,19 @@
       <c r="H81" t="n">
         <v>1921.46</v>
       </c>
-      <c r="O81" t="n">
+      <c r="J81" t="n">
+        <v>2193</v>
+      </c>
+      <c r="P81" t="n">
         <v>97.29000000000001</v>
       </c>
-      <c r="P81" t="n">
-        <v>674.16</v>
-      </c>
       <c r="Q81" t="n">
-        <v>50.87</v>
+        <v>674.16</v>
       </c>
       <c r="R81" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S81" t="n">
         <v>2743.78</v>
       </c>
     </row>
@@ -2297,16 +2542,19 @@
       <c r="H82" t="n">
         <v>1921.46</v>
       </c>
-      <c r="O82" t="n">
+      <c r="J82" t="n">
+        <v>2174</v>
+      </c>
+      <c r="P82" t="n">
         <v>97.29000000000001</v>
       </c>
-      <c r="P82" t="n">
-        <v>674.16</v>
-      </c>
       <c r="Q82" t="n">
-        <v>50.87</v>
+        <v>674.16</v>
       </c>
       <c r="R82" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S82" t="n">
         <v>2743.78</v>
       </c>
     </row>
@@ -2320,16 +2568,19 @@
       <c r="H83" t="n">
         <v>1921.46</v>
       </c>
-      <c r="O83" t="n">
+      <c r="J83" t="n">
+        <v>2056</v>
+      </c>
+      <c r="P83" t="n">
         <v>97.29000000000001</v>
       </c>
-      <c r="P83" t="n">
-        <v>674.16</v>
-      </c>
       <c r="Q83" t="n">
-        <v>50.87</v>
+        <v>674.16</v>
       </c>
       <c r="R83" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S83" t="n">
         <v>2743.78</v>
       </c>
     </row>
@@ -2343,16 +2594,19 @@
       <c r="H84" t="n">
         <v>1921.46</v>
       </c>
-      <c r="O84" t="n">
+      <c r="J84" t="n">
+        <v>1852</v>
+      </c>
+      <c r="P84" t="n">
         <v>97.29000000000001</v>
       </c>
-      <c r="P84" t="n">
-        <v>674.16</v>
-      </c>
       <c r="Q84" t="n">
-        <v>50.87</v>
+        <v>674.16</v>
       </c>
       <c r="R84" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S84" t="n">
         <v>2743.78</v>
       </c>
     </row>
@@ -2366,16 +2620,19 @@
       <c r="H85" t="n">
         <v>1921.46</v>
       </c>
-      <c r="O85" t="n">
+      <c r="J85" t="n">
+        <v>1846</v>
+      </c>
+      <c r="P85" t="n">
         <v>97.29000000000001</v>
       </c>
-      <c r="P85" t="n">
-        <v>674.16</v>
-      </c>
       <c r="Q85" t="n">
-        <v>50.87</v>
+        <v>674.16</v>
       </c>
       <c r="R85" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S85" t="n">
         <v>2743.78</v>
       </c>
     </row>
@@ -2389,16 +2646,19 @@
       <c r="H86" t="n">
         <v>2061.41</v>
       </c>
-      <c r="O86" t="n">
+      <c r="J86" t="n">
+        <v>2090</v>
+      </c>
+      <c r="P86" t="n">
         <v>109.23</v>
       </c>
-      <c r="P86" t="n">
-        <v>674.16</v>
-      </c>
       <c r="Q86" t="n">
-        <v>50.87</v>
+        <v>674.16</v>
       </c>
       <c r="R86" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S86" t="n">
         <v>2895.67</v>
       </c>
     </row>
@@ -2412,16 +2672,19 @@
       <c r="H87" t="n">
         <v>2061.41</v>
       </c>
-      <c r="O87" t="n">
+      <c r="J87" t="n">
+        <v>2128</v>
+      </c>
+      <c r="P87" t="n">
         <v>109.23</v>
       </c>
-      <c r="P87" t="n">
-        <v>674.16</v>
-      </c>
       <c r="Q87" t="n">
-        <v>50.87</v>
+        <v>674.16</v>
       </c>
       <c r="R87" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S87" t="n">
         <v>2895.67</v>
       </c>
     </row>
@@ -2435,16 +2698,19 @@
       <c r="H88" t="n">
         <v>2061.41</v>
       </c>
-      <c r="O88" t="n">
+      <c r="J88" t="n">
+        <v>2078</v>
+      </c>
+      <c r="P88" t="n">
         <v>109.23</v>
       </c>
-      <c r="P88" t="n">
-        <v>674.16</v>
-      </c>
       <c r="Q88" t="n">
-        <v>50.87</v>
+        <v>674.16</v>
       </c>
       <c r="R88" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S88" t="n">
         <v>2895.67</v>
       </c>
     </row>
@@ -2458,16 +2724,19 @@
       <c r="H89" t="n">
         <v>2061.41</v>
       </c>
-      <c r="O89" t="n">
+      <c r="J89" t="n">
+        <v>2141</v>
+      </c>
+      <c r="P89" t="n">
         <v>109.23</v>
       </c>
-      <c r="P89" t="n">
-        <v>674.16</v>
-      </c>
       <c r="Q89" t="n">
-        <v>50.87</v>
+        <v>674.16</v>
       </c>
       <c r="R89" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S89" t="n">
         <v>2895.67</v>
       </c>
     </row>
@@ -2481,16 +2750,19 @@
       <c r="H90" t="n">
         <v>2061.41</v>
       </c>
-      <c r="O90" t="n">
+      <c r="J90" t="n">
+        <v>2078</v>
+      </c>
+      <c r="P90" t="n">
         <v>109.23</v>
       </c>
-      <c r="P90" t="n">
-        <v>674.16</v>
-      </c>
       <c r="Q90" t="n">
-        <v>50.87</v>
+        <v>674.16</v>
       </c>
       <c r="R90" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S90" t="n">
         <v>2895.67</v>
       </c>
     </row>
@@ -2504,16 +2776,19 @@
       <c r="H91" t="n">
         <v>2077.9</v>
       </c>
-      <c r="O91" t="n">
+      <c r="J91" t="n">
+        <v>1913</v>
+      </c>
+      <c r="P91" t="n">
         <v>109.23</v>
       </c>
-      <c r="P91" t="n">
-        <v>674.16</v>
-      </c>
       <c r="Q91" t="n">
-        <v>50.87</v>
+        <v>674.16</v>
       </c>
       <c r="R91" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S91" t="n">
         <v>2912.16</v>
       </c>
     </row>
@@ -2527,16 +2802,19 @@
       <c r="H92" t="n">
         <v>2077.9</v>
       </c>
-      <c r="O92" t="n">
+      <c r="J92" t="n">
+        <v>2321</v>
+      </c>
+      <c r="P92" t="n">
         <v>109.23</v>
       </c>
-      <c r="P92" t="n">
-        <v>674.16</v>
-      </c>
       <c r="Q92" t="n">
-        <v>50.87</v>
+        <v>674.16</v>
       </c>
       <c r="R92" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S92" t="n">
         <v>2912.16</v>
       </c>
     </row>
@@ -2550,16 +2828,19 @@
       <c r="H93" t="n">
         <v>2077.9</v>
       </c>
-      <c r="O93" t="n">
+      <c r="J93" t="n">
+        <v>2087</v>
+      </c>
+      <c r="P93" t="n">
         <v>109.23</v>
       </c>
-      <c r="P93" t="n">
-        <v>674.16</v>
-      </c>
       <c r="Q93" t="n">
-        <v>50.87</v>
+        <v>674.16</v>
       </c>
       <c r="R93" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S93" t="n">
         <v>2912.16</v>
       </c>
     </row>
@@ -2573,16 +2854,19 @@
       <c r="H94" t="n">
         <v>2077.9</v>
       </c>
-      <c r="O94" t="n">
+      <c r="J94" t="n">
+        <v>2302</v>
+      </c>
+      <c r="P94" t="n">
         <v>109.23</v>
       </c>
-      <c r="P94" t="n">
-        <v>674.16</v>
-      </c>
       <c r="Q94" t="n">
-        <v>50.87</v>
+        <v>674.16</v>
       </c>
       <c r="R94" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="S94" t="n">
         <v>2912.16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add bin directory, refactor to prepare details extraction
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -451,6 +451,7 @@
     <col width="26" customWidth="1" min="22" max="22"/>
     <col width="40" customWidth="1" min="23" max="23"/>
     <col width="22" customWidth="1" min="24" max="24"/>
+    <col width="12" customWidth="1" min="25" max="25"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -574,6 +575,11 @@
           <t>legenda_rol</t>
         </is>
       </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>detail</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
@@ -642,6 +648,7 @@
       <c r="X2" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y2" s="1" t="n"/>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
@@ -710,6 +717,7 @@
       <c r="X3" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y3" s="1" t="n"/>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
@@ -778,6 +786,7 @@
       <c r="X4" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y4" s="1" t="n"/>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
@@ -846,6 +855,7 @@
       <c r="X5" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y5" s="1" t="n"/>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
@@ -914,6 +924,7 @@
       <c r="X6" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y6" s="1" t="n"/>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
@@ -982,6 +993,7 @@
       <c r="X7" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y7" s="1" t="n"/>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
@@ -1050,6 +1062,7 @@
       <c r="X8" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y8" s="1" t="n"/>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
@@ -1118,6 +1131,7 @@
       <c r="X9" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y9" s="1" t="n"/>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
@@ -1186,6 +1200,7 @@
       <c r="X10" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y10" s="1" t="n"/>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
@@ -1254,6 +1269,7 @@
       <c r="X11" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y11" s="1" t="n"/>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
@@ -1322,6 +1338,7 @@
       <c r="X12" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y12" s="1" t="n"/>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
@@ -1390,6 +1407,7 @@
       <c r="X13" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y13" s="1" t="n"/>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
@@ -1458,6 +1476,7 @@
       <c r="X14" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y14" s="1" t="n"/>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
@@ -1526,6 +1545,7 @@
       <c r="X15" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y15" s="1" t="n"/>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
@@ -1594,6 +1614,7 @@
       <c r="X16" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y16" s="1" t="n"/>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
@@ -1662,6 +1683,7 @@
       <c r="X17" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y17" s="1" t="n"/>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
@@ -1730,6 +1752,7 @@
       <c r="X18" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y18" s="1" t="n"/>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
@@ -1798,6 +1821,7 @@
       <c r="X19" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y19" s="1" t="n"/>
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
@@ -1866,6 +1890,7 @@
       <c r="X20" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y20" s="1" t="n"/>
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
@@ -1934,6 +1959,7 @@
       <c r="X21" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y21" s="1" t="n"/>
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
@@ -2002,6 +2028,7 @@
       <c r="X22" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y22" s="1" t="n"/>
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
@@ -2070,6 +2097,7 @@
       <c r="X23" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y23" s="1" t="n"/>
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
@@ -2138,6 +2166,7 @@
       <c r="X24" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y24" s="1" t="n"/>
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
@@ -2206,6 +2235,7 @@
       <c r="X25" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y25" s="1" t="n"/>
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
@@ -2274,6 +2304,7 @@
       <c r="X26" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y26" s="1" t="n"/>
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
@@ -2342,6 +2373,7 @@
       <c r="X27" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y27" s="1" t="n"/>
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
@@ -2410,6 +2442,7 @@
       <c r="X28" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y28" s="1" t="n"/>
     </row>
     <row r="29">
       <c r="A29" s="2" t="n">
@@ -2478,6 +2511,7 @@
       <c r="X29" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y29" s="1" t="n"/>
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
@@ -2546,6 +2580,7 @@
       <c r="X30" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y30" s="1" t="n"/>
     </row>
     <row r="31">
       <c r="A31" s="2" t="n">
@@ -2614,6 +2649,7 @@
       <c r="X31" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y31" s="1" t="n"/>
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
@@ -2682,6 +2718,7 @@
       <c r="X32" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y32" s="1" t="n"/>
     </row>
     <row r="33">
       <c r="A33" s="2" t="n">
@@ -2750,6 +2787,7 @@
       <c r="X33" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y33" s="1" t="n"/>
     </row>
     <row r="34">
       <c r="A34" s="2" t="n">
@@ -2818,6 +2856,7 @@
       <c r="X34" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y34" s="1" t="n"/>
     </row>
     <row r="35">
       <c r="A35" s="2" t="n">
@@ -2886,6 +2925,7 @@
       <c r="X35" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y35" s="1" t="n"/>
     </row>
     <row r="36">
       <c r="A36" s="2" t="n">
@@ -2954,6 +2994,7 @@
       <c r="X36" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y36" s="1" t="n"/>
     </row>
     <row r="37">
       <c r="A37" s="2" t="n">
@@ -3022,6 +3063,7 @@
       <c r="X37" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y37" s="1" t="n"/>
     </row>
     <row r="38">
       <c r="A38" s="2" t="n">
@@ -3090,6 +3132,7 @@
       <c r="X38" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y38" s="1" t="n"/>
     </row>
     <row r="39">
       <c r="A39" s="2" t="n">
@@ -3158,6 +3201,7 @@
       <c r="X39" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y39" s="1" t="n"/>
     </row>
     <row r="40">
       <c r="A40" s="2" t="n">
@@ -3226,6 +3270,7 @@
       <c r="X40" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y40" s="1" t="n"/>
     </row>
     <row r="41">
       <c r="A41" s="2" t="n">
@@ -3294,6 +3339,7 @@
       <c r="X41" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y41" s="1" t="n"/>
     </row>
     <row r="42">
       <c r="A42" s="2" t="n">
@@ -3362,6 +3408,7 @@
       <c r="X42" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y42" s="1" t="n"/>
     </row>
     <row r="43">
       <c r="A43" s="2" t="n">
@@ -3430,6 +3477,7 @@
       <c r="X43" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y43" s="1" t="n"/>
     </row>
     <row r="44">
       <c r="A44" s="2" t="n">
@@ -3498,6 +3546,7 @@
       <c r="X44" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y44" s="1" t="n"/>
     </row>
     <row r="45">
       <c r="A45" s="2" t="n">
@@ -3566,6 +3615,7 @@
       <c r="X45" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y45" s="1" t="n"/>
     </row>
     <row r="46">
       <c r="A46" s="2" t="n">
@@ -3634,6 +3684,7 @@
       <c r="X46" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y46" s="1" t="n"/>
     </row>
     <row r="47">
       <c r="A47" s="2" t="n">
@@ -3702,6 +3753,7 @@
       <c r="X47" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y47" s="1" t="n"/>
     </row>
     <row r="48">
       <c r="A48" s="2" t="n">
@@ -3770,6 +3822,7 @@
       <c r="X48" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y48" s="1" t="n"/>
     </row>
     <row r="49">
       <c r="A49" s="2" t="n">
@@ -3838,6 +3891,7 @@
       <c r="X49" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y49" s="1" t="n"/>
     </row>
     <row r="50">
       <c r="A50" s="2" t="n">
@@ -3906,6 +3960,7 @@
       <c r="X50" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y50" s="1" t="n"/>
     </row>
     <row r="51">
       <c r="A51" s="2" t="n">
@@ -3974,6 +4029,7 @@
       <c r="X51" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y51" s="1" t="n"/>
     </row>
     <row r="52">
       <c r="A52" s="2" t="n">
@@ -4042,6 +4098,7 @@
       <c r="X52" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y52" s="1" t="n"/>
     </row>
     <row r="53">
       <c r="A53" s="2" t="n">
@@ -4110,6 +4167,7 @@
       <c r="X53" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y53" s="1" t="n"/>
     </row>
     <row r="54">
       <c r="A54" s="2" t="n">
@@ -4178,6 +4236,7 @@
       <c r="X54" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y54" s="1" t="n"/>
     </row>
     <row r="55">
       <c r="A55" s="2" t="n">
@@ -4246,6 +4305,7 @@
       <c r="X55" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y55" s="1" t="n"/>
     </row>
     <row r="56">
       <c r="A56" s="2" t="n">
@@ -4314,6 +4374,7 @@
       <c r="X56" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y56" s="1" t="n"/>
     </row>
     <row r="57">
       <c r="A57" s="2" t="n">
@@ -4382,6 +4443,7 @@
       <c r="X57" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y57" s="1" t="n"/>
     </row>
     <row r="58">
       <c r="A58" s="2" t="n">
@@ -4450,6 +4512,7 @@
       <c r="X58" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="Y58" s="1" t="n"/>
     </row>
     <row r="59">
       <c r="A59" s="2" t="n">
@@ -4518,6 +4581,7 @@
       <c r="X59" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y59" s="1" t="n"/>
     </row>
     <row r="60">
       <c r="A60" s="2" t="n">
@@ -4586,6 +4650,7 @@
       <c r="X60" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y60" s="1" t="n"/>
     </row>
     <row r="61">
       <c r="A61" s="2" t="n">
@@ -4654,6 +4719,7 @@
       <c r="X61" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y61" s="1" t="n"/>
     </row>
     <row r="62">
       <c r="A62" s="2" t="n">
@@ -4722,6 +4788,7 @@
       <c r="X62" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y62" s="1" t="n"/>
     </row>
     <row r="63">
       <c r="A63" s="2" t="n">
@@ -4790,6 +4857,7 @@
       <c r="X63" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y63" s="1" t="n"/>
     </row>
     <row r="64">
       <c r="A64" s="2" t="n">
@@ -4858,6 +4926,7 @@
       <c r="X64" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y64" s="1" t="n"/>
     </row>
     <row r="65">
       <c r="A65" s="2" t="n">
@@ -4926,6 +4995,7 @@
       <c r="X65" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y65" s="1" t="n"/>
     </row>
     <row r="66">
       <c r="A66" s="2" t="n">
@@ -4994,6 +5064,7 @@
       <c r="X66" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="Y66" s="1" t="n"/>
     </row>
     <row r="67">
       <c r="A67" s="2" t="n">
@@ -5062,6 +5133,7 @@
       <c r="X67" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="Y67" s="1" t="n"/>
     </row>
     <row r="68">
       <c r="A68" s="2" t="n">
@@ -5130,6 +5202,7 @@
       <c r="X68" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y68" s="1" t="n"/>
     </row>
     <row r="69">
       <c r="A69" s="2" t="n">
@@ -5198,6 +5271,7 @@
       <c r="X69" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y69" s="1" t="n"/>
     </row>
     <row r="70">
       <c r="A70" s="2" t="n">
@@ -5266,6 +5340,7 @@
       <c r="X70" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y70" s="1" t="n"/>
     </row>
     <row r="71">
       <c r="A71" s="2" t="n">
@@ -5334,6 +5409,7 @@
       <c r="X71" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y71" s="1" t="n"/>
     </row>
     <row r="72">
       <c r="A72" s="2" t="n">
@@ -5402,6 +5478,7 @@
       <c r="X72" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y72" s="1" t="n"/>
     </row>
     <row r="73">
       <c r="A73" s="2" t="n">
@@ -5470,6 +5547,7 @@
       <c r="X73" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y73" s="1" t="n"/>
     </row>
     <row r="74">
       <c r="A74" s="2" t="n">
@@ -5538,6 +5616,7 @@
       <c r="X74" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y74" s="1" t="n"/>
     </row>
     <row r="75">
       <c r="A75" s="2" t="n">
@@ -5606,6 +5685,7 @@
       <c r="X75" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y75" s="1" t="n"/>
     </row>
     <row r="76">
       <c r="A76" s="2" t="n">
@@ -5674,6 +5754,7 @@
       <c r="X76" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y76" s="1" t="n"/>
     </row>
     <row r="77">
       <c r="A77" s="2" t="n">
@@ -5742,6 +5823,7 @@
       <c r="X77" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y77" s="1" t="n"/>
     </row>
     <row r="78">
       <c r="A78" s="2" t="n">
@@ -5810,6 +5892,7 @@
       <c r="X78" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y78" s="1" t="n"/>
     </row>
     <row r="79">
       <c r="A79" s="2" t="n">
@@ -5878,6 +5961,7 @@
       <c r="X79" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y79" s="1" t="n"/>
     </row>
     <row r="80">
       <c r="A80" s="2" t="n">
@@ -5946,6 +6030,7 @@
       <c r="X80" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="Y80" s="1" t="n"/>
     </row>
     <row r="81">
       <c r="A81" s="2" t="n">
@@ -6014,6 +6099,7 @@
       <c r="X81" s="3" t="n">
         <v>2</v>
       </c>
+      <c r="Y81" s="1" t="n"/>
     </row>
     <row r="82">
       <c r="A82" s="2" t="n">
@@ -6082,6 +6168,7 @@
       <c r="X82" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y82" s="1" t="n"/>
     </row>
     <row r="83">
       <c r="A83" s="2" t="n">
@@ -6150,6 +6237,7 @@
       <c r="X83" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y83" s="1" t="n"/>
     </row>
     <row r="84">
       <c r="A84" s="2" t="n">
@@ -6218,6 +6306,7 @@
       <c r="X84" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y84" s="1" t="n"/>
     </row>
     <row r="85">
       <c r="A85" s="2" t="n">
@@ -6286,6 +6375,7 @@
       <c r="X85" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y85" s="1" t="n"/>
     </row>
     <row r="86">
       <c r="A86" s="2" t="n">
@@ -6354,6 +6444,7 @@
       <c r="X86" s="3" t="n">
         <v>2</v>
       </c>
+      <c r="Y86" s="1" t="n"/>
     </row>
     <row r="87">
       <c r="A87" s="2" t="n">
@@ -6422,6 +6513,7 @@
       <c r="X87" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y87" s="1" t="n"/>
     </row>
     <row r="88">
       <c r="A88" s="2" t="n">
@@ -6490,6 +6582,7 @@
       <c r="X88" s="3" t="n">
         <v>3</v>
       </c>
+      <c r="Y88" s="1" t="n"/>
     </row>
     <row r="89">
       <c r="A89" s="2" t="n">
@@ -6558,6 +6651,7 @@
       <c r="X89" s="3" t="n">
         <v>48</v>
       </c>
+      <c r="Y89" s="1" t="n"/>
     </row>
     <row r="90">
       <c r="A90" s="2" t="n">
@@ -6626,6 +6720,7 @@
       <c r="X90" s="3" t="n">
         <v>32</v>
       </c>
+      <c r="Y90" s="1" t="n"/>
     </row>
     <row r="91">
       <c r="A91" s="2" t="n">
@@ -6694,6 +6789,7 @@
       <c r="X91" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y91" s="1" t="n"/>
     </row>
     <row r="92">
       <c r="A92" s="2" t="n">
@@ -6762,6 +6858,7 @@
       <c r="X92" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="Y92" s="1" t="n"/>
     </row>
     <row r="93">
       <c r="A93" s="2" t="n">
@@ -6830,6 +6927,7 @@
       <c r="X93" s="3" t="n">
         <v>48</v>
       </c>
+      <c r="Y93" s="1" t="n"/>
     </row>
     <row r="94">
       <c r="A94" s="2" t="n">
@@ -6898,6 +6996,7 @@
       <c r="X94" s="3" t="n">
         <v>30</v>
       </c>
+      <c r="Y94" s="1" t="n"/>
     </row>
     <row r="95">
       <c r="A95" s="2" t="n">
@@ -6966,6 +7065,7 @@
       <c r="X95" s="3" t="n">
         <v>2</v>
       </c>
+      <c r="Y95" s="1" t="n"/>
     </row>
     <row r="96">
       <c r="A96" s="2" t="n">
@@ -7034,6 +7134,7 @@
       <c r="X96" s="3" t="n">
         <v>32</v>
       </c>
+      <c r="Y96" s="1" t="n"/>
     </row>
     <row r="97">
       <c r="A97" s="2" t="n">
@@ -7102,6 +7203,7 @@
       <c r="X97" s="3" t="n">
         <v>16</v>
       </c>
+      <c r="Y97" s="1" t="n"/>
     </row>
     <row r="98">
       <c r="A98" s="2" t="n">
@@ -7170,6 +7272,7 @@
       <c r="X98" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y98" s="1" t="n"/>
     </row>
     <row r="99">
       <c r="A99" s="2" t="n">
@@ -7238,6 +7341,7 @@
       <c r="X99" s="3" t="n">
         <v>56</v>
       </c>
+      <c r="Y99" s="1" t="n"/>
     </row>
     <row r="100">
       <c r="A100" s="2" t="n">
@@ -7306,6 +7410,7 @@
       <c r="X100" s="3" t="n">
         <v>16</v>
       </c>
+      <c r="Y100" s="1" t="n"/>
     </row>
     <row r="101">
       <c r="A101" s="2" t="n">
@@ -7374,6 +7479,7 @@
       <c r="X101" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y101" s="1" t="n"/>
     </row>
     <row r="102">
       <c r="A102" s="2" t="n">
@@ -7442,6 +7548,7 @@
       <c r="X102" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y102" s="1" t="n"/>
     </row>
     <row r="103">
       <c r="A103" s="2" t="n">
@@ -7510,6 +7617,7 @@
       <c r="X103" s="3" t="n">
         <v>32</v>
       </c>
+      <c r="Y103" s="1" t="n"/>
     </row>
     <row r="104">
       <c r="A104" s="2" t="n">
@@ -7578,6 +7686,7 @@
       <c r="X104" s="3" t="n">
         <v>32</v>
       </c>
+      <c r="Y104" s="1" t="n"/>
     </row>
     <row r="105">
       <c r="A105" s="2" t="n">
@@ -7646,6 +7755,7 @@
       <c r="X105" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y105" s="1" t="n"/>
     </row>
     <row r="106">
       <c r="A106" s="2" t="n">
@@ -7714,6 +7824,7 @@
       <c r="X106" s="3" t="n">
         <v>64</v>
       </c>
+      <c r="Y106" s="1" t="n"/>
     </row>
     <row r="107">
       <c r="A107" s="2" t="n">
@@ -7782,6 +7893,7 @@
       <c r="X107" s="3" t="n">
         <v>56</v>
       </c>
+      <c r="Y107" s="1" t="n"/>
     </row>
     <row r="108">
       <c r="A108" s="2" t="n">
@@ -7850,6 +7962,7 @@
       <c r="X108" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y108" s="1" t="n"/>
     </row>
     <row r="109">
       <c r="A109" s="2" t="n">
@@ -7918,6 +8031,7 @@
       <c r="X109" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y109" s="1" t="n"/>
     </row>
     <row r="110">
       <c r="A110" s="2" t="n">
@@ -7986,6 +8100,7 @@
       <c r="X110" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y110" s="1" t="n"/>
     </row>
     <row r="111">
       <c r="A111" s="2" t="n">
@@ -8054,6 +8169,7 @@
       <c r="X111" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="Y111" s="1" t="n"/>
     </row>
     <row r="112">
       <c r="A112" s="2" t="n">
@@ -8122,6 +8238,76 @@
       <c r="X112" s="3" t="n">
         <v>50</v>
       </c>
+      <c r="Y112" s="1" t="n"/>
+    </row>
+    <row r="113">
+      <c r="A113" s="2" t="n">
+        <v>44228</v>
+      </c>
+      <c r="B113" s="3" t="n"/>
+      <c r="C113" s="3" t="n"/>
+      <c r="D113" s="3" t="n"/>
+      <c r="E113" s="4" t="n">
+        <v>2092.45</v>
+      </c>
+      <c r="F113" s="4" t="n">
+        <v>145.64</v>
+      </c>
+      <c r="G113" s="4" t="n">
+        <v>50.87</v>
+      </c>
+      <c r="H113" s="4" t="n">
+        <v>674.16</v>
+      </c>
+      <c r="I113" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J113" s="4" t="n">
+        <v>2963.12</v>
+      </c>
+      <c r="K113" s="3" t="n">
+        <v>35.18</v>
+      </c>
+      <c r="L113" s="3" t="n">
+        <v>3.34</v>
+      </c>
+      <c r="M113" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N113" s="3" t="n">
+        <v>38.52</v>
+      </c>
+      <c r="O113" s="3" t="n">
+        <v>246.68</v>
+      </c>
+      <c r="P113" s="3" t="n">
+        <v>17.34</v>
+      </c>
+      <c r="Q113" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="R113" s="3" t="n">
+        <v>264.02</v>
+      </c>
+      <c r="S113" s="4" t="n">
+        <v>2140</v>
+      </c>
+      <c r="T113" s="3" t="n">
+        <v>117</v>
+      </c>
+      <c r="U113" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="V113" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W113" s="3" t="n">
+        <v>64.5</v>
+      </c>
+      <c r="X113" s="3" t="n">
+        <v>35</v>
+      </c>
+      <c r="Y113" s="1" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>